<commit_message>
Implemented critical hours w afternoon/overnight diurnal FFMC
</commit_message>
<xml_diff>
--- a/api/app/data/diurnalFFMC_redbook.xlsx
+++ b/api/app/data/diurnalFFMC_redbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awilliam/Desktop/wps/api/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DA37596-CD0B-134B-9025-C63B4C0F34A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1BF134E-E3A2-A244-A5C2-F9039BDAB74D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32800" yWindow="1720" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2720" yWindow="2720" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="morning" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>0-68</t>
   </si>
@@ -84,30 +84,6 @@
   </si>
   <si>
     <t>52-100</t>
-  </si>
-  <si>
-    <t>0000</t>
-  </si>
-  <si>
-    <t>0100</t>
-  </si>
-  <si>
-    <t>0200</t>
-  </si>
-  <si>
-    <t>0300</t>
-  </si>
-  <si>
-    <t>0400</t>
-  </si>
-  <si>
-    <t>0500</t>
-  </si>
-  <si>
-    <t>0600</t>
-  </si>
-  <si>
-    <t>0700</t>
   </si>
 </sst>
 </file>
@@ -591,9 +567,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3161,68 +3138,68 @@
   <dimension ref="A1:S32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T32" sqref="T32"/>
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A1">
-        <v>1300</v>
-      </c>
-      <c r="B1">
-        <v>1400</v>
-      </c>
-      <c r="C1">
-        <v>1500</v>
-      </c>
-      <c r="D1">
-        <v>1600</v>
-      </c>
-      <c r="E1">
-        <v>1700</v>
-      </c>
-      <c r="F1">
-        <v>1800</v>
-      </c>
-      <c r="G1">
-        <v>1900</v>
-      </c>
-      <c r="H1">
-        <v>2000</v>
-      </c>
-      <c r="I1">
-        <v>2100</v>
-      </c>
-      <c r="J1">
-        <v>2200</v>
-      </c>
-      <c r="K1">
-        <v>2300</v>
-      </c>
-      <c r="L1" s="1" t="s">
+      <c r="A1" s="2">
+        <v>13</v>
+      </c>
+      <c r="B1" s="2">
+        <v>14</v>
+      </c>
+      <c r="C1" s="2">
+        <v>15</v>
+      </c>
+      <c r="D1" s="2">
+        <v>16</v>
+      </c>
+      <c r="E1" s="2">
+        <v>17</v>
+      </c>
+      <c r="F1" s="2">
+        <v>18</v>
+      </c>
+      <c r="G1" s="2">
+        <v>19</v>
+      </c>
+      <c r="H1" s="2">
+        <v>20</v>
+      </c>
+      <c r="I1" s="2">
         <v>21</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="J1" s="2">
         <v>22</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="K1" s="2">
         <v>23</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>28</v>
+      <c r="L1" s="1">
+        <v>0</v>
+      </c>
+      <c r="M1" s="1">
+        <v>1</v>
+      </c>
+      <c r="N1" s="1">
+        <v>2</v>
+      </c>
+      <c r="O1" s="1">
+        <v>3</v>
+      </c>
+      <c r="P1" s="1">
+        <v>4</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>5</v>
+      </c>
+      <c r="R1" s="1">
+        <v>6</v>
+      </c>
+      <c r="S1" s="1">
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">

</xml_diff>